<commit_message>
heading back to ish on 3/5
</commit_message>
<xml_diff>
--- a/201-8 (W25)/week 3 constant accelaration/lab 3 workbook.xlsx
+++ b/201-8 (W25)/week 3 constant accelaration/lab 3 workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlatza\Documents\winter2025\201-8 (W25)\week 3 constant accelaration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2648B48C-7FA0-45CD-845F-403F9B080F8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B02714-92EE-4111-BD07-45297220D7AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{275834FB-7F59-4A02-910C-776EFFF9C63A}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{275834FB-7F59-4A02-910C-776EFFF9C63A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,6 +255,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -583,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -594,70 +597,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -666,7 +618,79 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -701,6 +725,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Distance Vs Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -737,16 +786,11 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>displacement vs time</c:v>
-          </c:tx>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -756,95 +800,90 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$C$1:$C$11</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>|Δ x| (cm)</c:v>
+                  <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>190</c:v>
+                  <c:v>3.4666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>170</c:v>
+                  <c:v>3.2833333333333332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>3.1233333333333331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>130</c:v>
+                  <c:v>2.81</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>110</c:v>
+                  <c:v>2.66</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>2.5299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90</c:v>
+                  <c:v>2.39</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>2.27</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>60</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>2.1266666666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$1:$G$11</c:f>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4166666666666665</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4666666666666668</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2833333333333332</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1233333333333331</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.81</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.66</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5299999999999998</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.39</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.27</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.1266666666666665</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -852,11 +891,12 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D8DA-46CB-B23F-9BC4C8AD4958}"/>
+              <c16:uniqueId val="{00000000-3833-4453-AFA3-A677FD94DE72}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -864,113 +904,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1073754879"/>
-        <c:axId val="1352679359"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>|Δ x| (cm)</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:noFill/>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$2:$C$11</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
-                      <c:pt idx="0">
-                        <c:v>190</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>170</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>150</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>130</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>110</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>90</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>80</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>70</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>60</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-D8DA-46CB-B23F-9BC4C8AD4958}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:axId val="927247808"/>
+        <c:axId val="926306208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1073754879"/>
+        <c:axId val="927247808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -988,6 +929,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time, t (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1024,14 +1021,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1352679359"/>
+        <c:crossAx val="926306208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1352679359"/>
+        <c:axId val="926306208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="200"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1049,7 +1048,74 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Δ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>x (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1086,7 +1152,1282 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1073754879"/>
+        <c:crossAx val="927247808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Displacement</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>  Vs Time Squared</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.55689020122484689"/>
+                  <c:y val="0.69865740740740745"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = 13.7cm/s</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>x + 0.717cm</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>14.0625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.017777777777779</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.780277777777776</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7552111111111088</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8961000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0756000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4008999999999991</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7121000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.1528999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5227111111111107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C3F-44E0-AA91-97087257F370}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="779623872"/>
+        <c:axId val="922335520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="779623872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="15"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time Squared,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> t</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="50000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="50000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="922335520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="922335520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Displacement, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Δ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>x</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>  (cm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="779623872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Square</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>-Root of Displacement vs Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.52768722659667544"/>
+                  <c:y val="0.69865740740740745"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = 3.72 cm</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="30000">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>1/2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>/s x - 0.0039cm</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="30000">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>1/2</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2833333333333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1233333333333331</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1266666666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>13.784048752090222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.038404810405298</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.24744871391589</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.401754250991379</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.488088481701515</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4868329805051381</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9442719099991592</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.3666002653407556</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.745966692414834</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B01E-48D8-A32B-D40532E2AC50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="988492752"/>
+        <c:axId val="919113344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="988492752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time, t</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="919113344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="919113344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="14"/>
+          <c:min val="7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Displacemnet</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="30000"/>
+                  <a:t>1/2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Δ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>x</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="30000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>1/2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>, (cm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="30000"/>
+                  <a:t>1/2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="988492752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1182,6 +2523,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1698,27 +3119,1059 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>543892</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>113748</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>512734</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>74544</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>112644</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>225603</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152715</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47586D13-A89C-437A-B76C-C8ED365BEC77}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{611E2216-0248-4A47-AA0D-AE97BA4DC232}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1731,6 +4184,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>296202</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>113354</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121321</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE427028-1052-42B3-9419-4440664D92C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>215742</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>22243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>699683</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>30211</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1CFC3ED-EE79-488A-96D3-270EB4961B4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2038,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A231181-238B-4A5E-AD52-E06B8A1E6457}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2052,369 +4577,369 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
+      <c r="A2" s="23">
         <v>20</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="24">
         <v>210</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="25">
         <f>B2-A2</f>
         <v>190</v>
       </c>
-      <c r="D2" s="8">
-        <v>2.77</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="D2" s="11">
+        <v>3.77</v>
+      </c>
+      <c r="E2" s="12">
         <v>3.8</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="13">
         <v>3.68</v>
       </c>
-      <c r="G2" s="15">
-        <f>AVERAGE(D2:F2)</f>
-        <v>3.4166666666666665</v>
-      </c>
-      <c r="H2" s="24">
+      <c r="G2" s="35">
+        <f t="shared" ref="G2:G11" si="0">AVERAGE(D2:F2)</f>
+        <v>3.75</v>
+      </c>
+      <c r="H2" s="32">
         <f>G2^2</f>
-        <v>11.673611111111111</v>
-      </c>
-      <c r="I2" s="15">
+        <v>14.0625</v>
+      </c>
+      <c r="I2" s="25">
         <f>SQRT(C2)</f>
         <v>13.784048752090222</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="10">
+      <c r="A3" s="26">
         <v>20</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="27">
         <f>B2-20</f>
         <v>190</v>
       </c>
-      <c r="C3" s="16">
-        <f t="shared" ref="C3:C11" si="0">B3-A3</f>
+      <c r="C3" s="28">
+        <f t="shared" ref="C3:C11" si="1">B3-A3</f>
         <v>170</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="15">
         <v>3.48</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="16">
         <v>3.44</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="17">
         <v>3.48</v>
       </c>
-      <c r="G3" s="16">
-        <f t="shared" ref="G3:G11" si="1">AVERAGE(D3:F3)</f>
+      <c r="G3" s="18">
+        <f t="shared" si="0"/>
         <v>3.4666666666666668</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="33">
         <f t="shared" ref="H3:H11" si="2">G3^2</f>
         <v>12.017777777777779</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="28">
         <f t="shared" ref="I3:I11" si="3">SQRT(C3)</f>
         <v>13.038404810405298</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+      <c r="A4" s="23">
         <v>20</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="24">
         <f t="shared" ref="B4:B5" si="4">B3-20</f>
         <v>170</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="25">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="D4" s="11">
+        <v>3.27</v>
+      </c>
+      <c r="E4" s="12">
+        <v>3.26</v>
+      </c>
+      <c r="F4" s="13">
+        <v>3.32</v>
+      </c>
+      <c r="G4" s="14">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3.27</v>
-      </c>
-      <c r="E4" s="4">
-        <v>3.26</v>
-      </c>
-      <c r="F4" s="21">
-        <v>3.32</v>
-      </c>
-      <c r="G4" s="15">
-        <f t="shared" si="1"/>
         <v>3.2833333333333332</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="32">
         <f t="shared" si="2"/>
         <v>10.780277777777776</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="25">
         <f t="shared" si="3"/>
         <v>12.24744871391589</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
+      <c r="A5" s="26">
         <v>20</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="27">
         <f t="shared" si="4"/>
         <v>150</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="28">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="D5" s="15">
+        <v>3.03</v>
+      </c>
+      <c r="E5" s="16">
+        <v>3.16</v>
+      </c>
+      <c r="F5" s="17">
+        <v>3.18</v>
+      </c>
+      <c r="G5" s="18">
         <f t="shared" si="0"/>
-        <v>130</v>
-      </c>
-      <c r="D5" s="10">
-        <v>3.03</v>
-      </c>
-      <c r="E5" s="5">
-        <v>3.16</v>
-      </c>
-      <c r="F5" s="22">
-        <v>3.18</v>
-      </c>
-      <c r="G5" s="16">
-        <f t="shared" si="1"/>
         <v>3.1233333333333331</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="33">
         <f t="shared" si="2"/>
         <v>9.7552111111111088</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="28">
         <f t="shared" si="3"/>
         <v>11.401754250991379</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
+      <c r="A6" s="23">
         <v>20</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="24">
         <f>B5-20</f>
         <v>130</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="25">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="D6" s="11">
+        <v>2.84</v>
+      </c>
+      <c r="E6" s="12">
+        <v>2.79</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2.8</v>
+      </c>
+      <c r="G6" s="14">
         <f t="shared" si="0"/>
-        <v>110</v>
-      </c>
-      <c r="D6" s="8">
-        <v>2.84</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2.79</v>
-      </c>
-      <c r="F6" s="21">
-        <v>2.8</v>
-      </c>
-      <c r="G6" s="15">
-        <f t="shared" si="1"/>
         <v>2.81</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="32">
         <f t="shared" si="2"/>
         <v>7.8961000000000006</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="25">
         <f t="shared" si="3"/>
         <v>10.488088481701515</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
+      <c r="A7" s="26">
         <v>20</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="27">
         <f>B6-10</f>
         <v>120</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="28">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="D7" s="15">
+        <v>2.65</v>
+      </c>
+      <c r="E7" s="16">
+        <v>2.64</v>
+      </c>
+      <c r="F7" s="17">
+        <v>2.69</v>
+      </c>
+      <c r="G7" s="18">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2.65</v>
-      </c>
-      <c r="E7" s="5">
-        <v>2.64</v>
-      </c>
-      <c r="F7" s="22">
-        <v>2.69</v>
-      </c>
-      <c r="G7" s="16">
-        <f t="shared" si="1"/>
         <v>2.66</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="33">
         <f t="shared" si="2"/>
         <v>7.0756000000000006</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="28">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
+      <c r="A8" s="23">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="24">
         <f t="shared" ref="B8:B11" si="5">B7-10</f>
         <v>110</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="25">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="E8" s="12">
+        <v>2.52</v>
+      </c>
+      <c r="F8" s="13">
+        <v>2.54</v>
+      </c>
+      <c r="G8" s="14">
         <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="D8" s="8">
         <v>2.5299999999999998</v>
       </c>
-      <c r="E8" s="4">
-        <v>2.52</v>
-      </c>
-      <c r="F8" s="21">
-        <v>2.54</v>
-      </c>
-      <c r="G8" s="15">
-        <f t="shared" si="1"/>
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="H8" s="24">
+      <c r="H8" s="32">
         <f t="shared" si="2"/>
         <v>6.4008999999999991</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="25">
         <f t="shared" si="3"/>
         <v>9.4868329805051381</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10">
+      <c r="A9" s="26">
         <v>20</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="27">
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="28">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="D9" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="E9" s="16">
+        <v>2.37</v>
+      </c>
+      <c r="F9" s="17">
+        <v>2.4</v>
+      </c>
+      <c r="G9" s="18">
         <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="D9" s="10">
-        <v>2.4</v>
-      </c>
-      <c r="E9" s="5">
-        <v>2.37</v>
-      </c>
-      <c r="F9" s="22">
-        <v>2.4</v>
-      </c>
-      <c r="G9" s="16">
-        <f t="shared" si="1"/>
         <v>2.39</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="33">
         <f t="shared" si="2"/>
         <v>5.7121000000000004</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="28">
         <f t="shared" si="3"/>
         <v>8.9442719099991592</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="8">
+      <c r="A10" s="23">
         <v>20</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="24">
         <f t="shared" si="5"/>
         <v>90</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="25">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F10" s="13">
+        <v>2.29</v>
+      </c>
+      <c r="G10" s="14">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="D10" s="8">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="F10" s="21">
-        <v>2.29</v>
-      </c>
-      <c r="G10" s="15">
-        <f t="shared" si="1"/>
         <v>2.27</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="32">
         <f t="shared" si="2"/>
         <v>5.1528999999999998</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="25">
         <f t="shared" si="3"/>
         <v>8.3666002653407556</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="12">
+      <c r="A11" s="29">
         <v>20</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="30">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="31">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2.08</v>
+      </c>
+      <c r="E11" s="20">
+        <v>2.13</v>
+      </c>
+      <c r="F11" s="21">
+        <v>2.17</v>
+      </c>
+      <c r="G11" s="22">
         <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="D11" s="12">
-        <v>2.08</v>
-      </c>
-      <c r="E11" s="19">
-        <v>2.13</v>
-      </c>
-      <c r="F11" s="23">
-        <v>2.17</v>
-      </c>
-      <c r="G11" s="17">
-        <f t="shared" si="1"/>
         <v>2.1266666666666665</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="34">
         <f t="shared" si="2"/>
         <v>4.5227111111111107</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="31">
         <f t="shared" si="3"/>
         <v>7.745966692414834</v>
       </c>

</xml_diff>

<commit_message>
preped for grading week 3 stuff
</commit_message>
<xml_diff>
--- a/201-8 (W25)/week 3 constant accelaration/lab 3 workbook.xlsx
+++ b/201-8 (W25)/week 3 constant accelaration/lab 3 workbook.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlatza\Documents\winter2025\201-8 (W25)\week 3 constant accelaration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B02714-92EE-4111-BD07-45297220D7AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE048371-FC8C-4FF4-B5EF-ABFE2480D2A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{275834FB-7F59-4A02-910C-776EFFF9C63A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{275834FB-7F59-4A02-910C-776EFFF9C63A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <r>
       <t>x</t>
@@ -250,13 +251,19 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>|Δ x| (cm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -586,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,31 +661,31 @@
     <xf numFmtId="2" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -691,6 +698,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -745,7 +770,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Distance Vs Time</a:t>
+              <a:t>Displacement Vs Time</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -896,7 +921,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2483,6 +2507,746 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2833333333333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1233333333333331</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1266666666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D464-48CC-B1ED-2A0ACE3FF385}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="411230511"/>
+        <c:axId val="548107695"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="411230511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="548107695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="548107695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411230511"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$2:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$L$2:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-39C0-495B-834E-8DF284FF54C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="599748463"/>
+        <c:axId val="548280335"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="599748463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="548280335"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="548280335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599748463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2603,6 +3367,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4151,20 +4995,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>512734</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>455584</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>225603</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152715</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>168453</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>51115</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4256,6 +6132,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>212725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>231775</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78C98585-1CD3-4ACE-B85F-C19ECE8157A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>103414</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>120653</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88903</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C519C5B8-B185-4535-BD94-25CC530985BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4561,22 +6514,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A231181-238B-4A5E-AD52-E06B8A1E6457}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="7.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="1" customWidth="1"/>
     <col min="4" max="6" width="7.6328125" style="1" customWidth="1"/>
     <col min="7" max="9" width="10.08984375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4604,8 +6557,14 @@
       <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="23">
         <v>20</v>
       </c>
@@ -4637,8 +6596,14 @@
         <f>SQRT(C2)</f>
         <v>13.784048752090222</v>
       </c>
+      <c r="K2" s="40">
+        <v>3.75</v>
+      </c>
+      <c r="L2" s="38">
+        <v>190</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="26">
         <v>20</v>
       </c>
@@ -4671,8 +6636,14 @@
         <f t="shared" ref="I3:I11" si="3">SQRT(C3)</f>
         <v>13.038404810405298</v>
       </c>
+      <c r="K3" s="40">
+        <v>3.4666666666666668</v>
+      </c>
+      <c r="L3" s="38">
+        <v>170</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="23">
         <v>20</v>
       </c>
@@ -4705,8 +6676,14 @@
         <f t="shared" si="3"/>
         <v>12.24744871391589</v>
       </c>
+      <c r="K4" s="40">
+        <v>3.2833333333333332</v>
+      </c>
+      <c r="L4" s="38">
+        <v>150</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26">
         <v>20</v>
       </c>
@@ -4739,8 +6716,14 @@
         <f t="shared" si="3"/>
         <v>11.401754250991379</v>
       </c>
+      <c r="K5" s="41">
+        <v>3.1233333333333331</v>
+      </c>
+      <c r="L5" s="39">
+        <v>130</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="23">
         <v>20</v>
       </c>
@@ -4773,8 +6756,14 @@
         <f t="shared" si="3"/>
         <v>10.488088481701515</v>
       </c>
+      <c r="K6" s="40">
+        <v>2.81</v>
+      </c>
+      <c r="L6" s="38">
+        <v>110</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>20</v>
       </c>
@@ -4807,8 +6796,14 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
+      <c r="K7" s="40">
+        <v>2.66</v>
+      </c>
+      <c r="L7" s="38">
+        <v>100</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="23">
         <v>20</v>
       </c>
@@ -4841,8 +6836,14 @@
         <f t="shared" si="3"/>
         <v>9.4868329805051381</v>
       </c>
+      <c r="K8" s="40">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="L8" s="38">
+        <v>90</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="26">
         <v>20</v>
       </c>
@@ -4875,8 +6876,14 @@
         <f t="shared" si="3"/>
         <v>8.9442719099991592</v>
       </c>
+      <c r="K9" s="41">
+        <v>2.39</v>
+      </c>
+      <c r="L9" s="39">
+        <v>80</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="23">
         <v>20</v>
       </c>
@@ -4909,8 +6916,14 @@
         <f t="shared" si="3"/>
         <v>8.3666002653407556</v>
       </c>
+      <c r="K10" s="40">
+        <v>2.27</v>
+      </c>
+      <c r="L10" s="38">
+        <v>70</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="29">
         <v>20</v>
       </c>
@@ -4942,6 +6955,17 @@
       <c r="I11" s="31">
         <f t="shared" si="3"/>
         <v>7.745966692414834</v>
+      </c>
+      <c r="K11" s="41">
+        <v>2.1266666666666665</v>
+      </c>
+      <c r="L11" s="39">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H13" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -4949,4 +6973,127 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F7DEF1-E864-4954-B9B4-FE39BAC69FBA}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>210</v>
+      </c>
+      <c r="C2">
+        <f>ABS(B2-A2)</f>
+        <v>190</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>190</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="0">ABS(B3-A3)</f>
+        <v>170</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>170</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>